<commit_message>
modified templates for ease readability when visualize
</commit_message>
<xml_diff>
--- a/data_raw/data/financial/balance_sheet_template.xlsx
+++ b/data_raw/data/financial/balance_sheet_template.xlsx
@@ -519,7 +519,7 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Current Assets</t>
+          <t xml:space="preserve">    Current Assets</t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr"/>
@@ -536,7 +536,7 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Cash</t>
+          <t xml:space="preserve">        Cash</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr"/>
@@ -553,7 +553,7 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Accounts receivable</t>
+          <t xml:space="preserve">        Accounts receivable</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr"/>
@@ -570,7 +570,7 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Inventory</t>
+          <t xml:space="preserve">        Inventory</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr"/>
@@ -587,7 +587,7 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Prepaid expenses</t>
+          <t xml:space="preserve">        Prepaid expenses</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr"/>
@@ -604,7 +604,7 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Short-term investments</t>
+          <t xml:space="preserve">        Short-term investments</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr"/>
@@ -621,7 +621,7 @@
       </c>
       <c r="B9" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Total current assets</t>
+          <t xml:space="preserve">    Total current assets</t>
         </is>
       </c>
       <c r="C9" s="5" t="inlineStr">
@@ -644,7 +644,7 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Fixed (Long-Term) Assets</t>
+          <t xml:space="preserve">    Fixed (Long-Term) Assets</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr"/>
@@ -661,7 +661,7 @@
       </c>
       <c r="B11" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Long-term investments</t>
+          <t xml:space="preserve">        Long-term investments</t>
         </is>
       </c>
       <c r="C11" s="4" t="inlineStr"/>
@@ -678,7 +678,7 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Property, plant, and equipment</t>
+          <t xml:space="preserve">        Property, plant, and equipment</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr"/>
@@ -695,7 +695,7 @@
       </c>
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    (Less accumulated depreciation)</t>
+          <t xml:space="preserve">        (Less accumulated depreciation)</t>
         </is>
       </c>
       <c r="C13" s="4" t="inlineStr"/>
@@ -712,7 +712,7 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Intangible assets</t>
+          <t xml:space="preserve">        Intangible assets</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr"/>
@@ -729,7 +729,7 @@
       </c>
       <c r="B15" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Total fixed assets</t>
+          <t xml:space="preserve">    Total fixed assets</t>
         </is>
       </c>
       <c r="C15" s="5" t="inlineStr">
@@ -752,7 +752,7 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Other Assets</t>
+          <t xml:space="preserve">    Other Assets</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr"/>
@@ -769,7 +769,7 @@
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Deferred income tax</t>
+          <t xml:space="preserve">        Deferred income tax</t>
         </is>
       </c>
       <c r="C17" s="4" t="inlineStr"/>
@@ -786,7 +786,7 @@
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Other</t>
+          <t xml:space="preserve">        Other</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr"/>
@@ -803,7 +803,7 @@
       </c>
       <c r="B19" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Total Other Assets</t>
+          <t xml:space="preserve">    Total Other Assets</t>
         </is>
       </c>
       <c r="C19" s="5" t="inlineStr">
@@ -884,7 +884,7 @@
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Current Liabilities</t>
+          <t xml:space="preserve">    Current Liabilities</t>
         </is>
       </c>
       <c r="C24" s="2" t="inlineStr"/>
@@ -901,7 +901,7 @@
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Accounts payable</t>
+          <t xml:space="preserve">        Accounts payable</t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr"/>
@@ -918,7 +918,7 @@
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Short-term loans</t>
+          <t xml:space="preserve">        Short-term loans</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr"/>
@@ -935,7 +935,7 @@
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Income taxes payable</t>
+          <t xml:space="preserve">        Income taxes payable</t>
         </is>
       </c>
       <c r="C27" s="4" t="inlineStr"/>
@@ -952,7 +952,7 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Accrued salaries and wages</t>
+          <t xml:space="preserve">        Accrued salaries and wages</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr"/>
@@ -969,7 +969,7 @@
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Unearned revenue</t>
+          <t xml:space="preserve">        Unearned revenue</t>
         </is>
       </c>
       <c r="C29" s="4" t="inlineStr"/>
@@ -986,7 +986,7 @@
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Current portion of long-term debt</t>
+          <t xml:space="preserve">        Current portion of long-term debt</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr"/>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="B31" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Total current liabilities</t>
+          <t xml:space="preserve">    Total current liabilities</t>
         </is>
       </c>
       <c r="C31" s="5" t="inlineStr">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Long-Term Liabilities</t>
+          <t xml:space="preserve">    Long-Term Liabilities</t>
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr"/>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Long-term debt</t>
+          <t xml:space="preserve">        Long-term debt</t>
         </is>
       </c>
       <c r="C33" s="4" t="inlineStr"/>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Deferred income tax</t>
+          <t xml:space="preserve">        Deferred income tax</t>
         </is>
       </c>
       <c r="C34" s="2" t="inlineStr"/>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Other</t>
+          <t xml:space="preserve">        Other</t>
         </is>
       </c>
       <c r="C35" s="4" t="inlineStr"/>
@@ -1094,7 +1094,7 @@
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Total long-term liabilities</t>
+          <t xml:space="preserve">    Total long-term liabilities</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="B37" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Owner's Equity</t>
+          <t xml:space="preserve">    Owner's Equity</t>
         </is>
       </c>
       <c r="C37" s="4" t="inlineStr"/>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Owner's investment</t>
+          <t xml:space="preserve">        Owner's investment</t>
         </is>
       </c>
       <c r="C38" s="2" t="inlineStr"/>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="B39" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Retained earnings</t>
+          <t xml:space="preserve">        Retained earnings</t>
         </is>
       </c>
       <c r="C39" s="4" t="inlineStr"/>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Other</t>
+          <t xml:space="preserve">        Other</t>
         </is>
       </c>
       <c r="C40" s="2" t="inlineStr"/>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="B41" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Total owner's equity</t>
+          <t xml:space="preserve">    Total owner's equity</t>
         </is>
       </c>
       <c r="C41" s="5" t="inlineStr">
@@ -1266,7 +1266,7 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>Debt Ratio (Total Liabilities / Total Assets)</t>
+          <t xml:space="preserve">    Debt Ratio (Total Liabilities / Total Assets)</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="B47" s="4" t="inlineStr">
         <is>
-          <t>Current Ratio (Current Assets / Current Liabilities)</t>
+          <t xml:space="preserve">    Current Ratio (Current Assets / Current Liabilities)</t>
         </is>
       </c>
       <c r="C47" s="5" t="inlineStr">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>Working Capital (Current Assets - Current Liabilities)</t>
+          <t xml:space="preserve">    Working Capital (Current Assets - Current Liabilities)</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
@@ -1335,7 +1335,7 @@
       </c>
       <c r="B49" s="5" t="inlineStr">
         <is>
-          <t>Assets-to-Equity Ratio (Total Assets / Owner's Equity)</t>
+          <t xml:space="preserve">    Assets-to-Equity Ratio (Total Assets / Owner's Equity)</t>
         </is>
       </c>
       <c r="C49" s="5" t="inlineStr">
@@ -1358,7 +1358,7 @@
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>Debt-to-Equity Ratio (Total Liabilities / Owner's Equity)</t>
+          <t xml:space="preserve">    Debt-to-Equity Ratio (Total Liabilities / Owner's Equity)</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">

</xml_diff>